<commit_message>
New pricing data entered and documentation on Excel was updated
</commit_message>
<xml_diff>
--- a/CustomerFiles/ProductHierarchy.xlsx
+++ b/CustomerFiles/ProductHierarchy.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10773" windowHeight="4593"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Product</t>
   </si>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,20 +422,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.29296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -463,157 +463,171 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="E4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B5">
-        <v>2</v>
-      </c>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>50</v>
-      </c>
-      <c r="E5">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>100</v>
-      </c>
-      <c r="E6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>1000</v>
       </c>
       <c r="E7">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>500000</v>
       </c>
-      <c r="E8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
+      <c r="E9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>10000</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="D10">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>20000</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
         <v>30000</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
         <v>40000</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>500000</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>1</v>
       </c>
     </row>
@@ -623,19 +637,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -643,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -651,7 +665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -659,7 +673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -667,7 +681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -675,7 +689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -689,19 +703,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -721,7 +735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -732,16 +746,16 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -752,16 +766,16 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E3">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -772,36 +786,36 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="E4">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="E5">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -809,19 +823,19 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="E6">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -829,10 +843,10 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>0.1</v>
@@ -841,27 +855,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>500000</v>
+        <v>100</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -872,56 +886,56 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>10000</v>
+        <v>500000</v>
       </c>
       <c r="E9">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="F9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="E10">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="F10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E11">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="F11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -929,19 +943,19 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E12">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -949,15 +963,35 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
+        <v>40000</v>
+      </c>
+      <c r="E13">
+        <v>0.6</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>500000</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New pricing for Drift put into customer files
</commit_message>
<xml_diff>
--- a/CustomerFiles/ProductHierarchy.xlsx
+++ b/CustomerFiles/ProductHierarchy.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +466,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -474,10 +474,10 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>360</v>
       </c>
       <c r="E3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -485,62 +485,68 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>250</v>
+        <v>1200</v>
       </c>
       <c r="E4">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
       <c r="C5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1000</v>
+        <v>25</v>
       </c>
       <c r="E5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>25</v>
-      </c>
-      <c r="E6">
-        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E7">
         <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
       <c r="C8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>500000</v>
       </c>
       <c r="E8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -549,85 +555,68 @@
         <v>1</v>
       </c>
       <c r="D9">
+        <v>10000</v>
+      </c>
+      <c r="E9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>20000</v>
+      </c>
+      <c r="E10">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>30000</v>
+      </c>
+      <c r="E11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>40000</v>
+      </c>
+      <c r="E12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>500000</v>
       </c>
-      <c r="E9">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>10000</v>
-      </c>
-      <c r="E10">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>20000</v>
-      </c>
-      <c r="E11">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>30000</v>
-      </c>
-      <c r="E12">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>40000</v>
-      </c>
       <c r="E13">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>500000</v>
-      </c>
-      <c r="E14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Plotting changes into Sales Sheet
</commit_message>
<xml_diff>
--- a/CustomerFiles/ProductHierarchy.xlsx
+++ b/CustomerFiles/ProductHierarchy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4590" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Product</t>
   </si>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
         <v>50</v>
       </c>
       <c r="E6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>100</v>
       </c>
       <c r="E7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -693,10 +693,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -755,10 +755,10 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>360</v>
       </c>
       <c r="E3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -775,10 +775,10 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>250</v>
+        <v>1200</v>
       </c>
       <c r="E4">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -789,16 +789,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -812,13 +812,13 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -832,13 +832,13 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -849,19 +849,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>500000</v>
       </c>
       <c r="E8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -875,13 +875,13 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>500000</v>
+        <v>10000</v>
       </c>
       <c r="E9">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -889,16 +889,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="E10">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -909,19 +909,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E11">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -932,13 +932,13 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E12">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -952,35 +952,15 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>40000</v>
+        <v>500000</v>
       </c>
       <c r="E13">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>500000</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
         <v>5</v>
       </c>
     </row>

</xml_diff>